<commit_message>
Edited a Check for B023 CFG Restart
Even though we may not use it.
</commit_message>
<xml_diff>
--- a/Example D20 XML/D20M++/FE D20 M++ QC Doc Rev 3 Template.xlsx
+++ b/Example D20 XML/D20M++/FE D20 M++ QC Doc Rev 3 Template.xlsx
@@ -20,12 +20,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'D20++ QC Doc'!$B$1:$L$223</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'D20++ QC Doc'!$8:$8</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="221">
   <si>
     <t>D20 ME,  MEII and MX QC Document</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>Message</t>
+  </si>
+  <si>
+    <t>Minimum 10 or 3 + # of DNP Devices</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1348,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1734,38 +1737,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1773,6 +1782,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1780,6 +1792,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1801,26 +1816,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3994,8 +4000,8 @@
   <dimension ref="A1:V229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <pane ySplit="8" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4011,11 +4017,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
     </row>
     <row r="2" spans="2:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
@@ -4108,7 +4114,7 @@
       <c r="E10" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="156"/>
+      <c r="F10" s="158"/>
       <c r="G10" s="30"/>
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
@@ -4146,7 +4152,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" s="78" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="150" t="s">
+      <c r="D13" s="156" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="67"/>
@@ -4162,7 +4168,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="147"/>
+      <c r="D14" s="157"/>
       <c r="E14" s="67"/>
       <c r="F14" s="68"/>
       <c r="H14" s="50"/>
@@ -4176,7 +4182,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="147"/>
+      <c r="D15" s="157"/>
       <c r="E15" s="67"/>
       <c r="F15" s="68"/>
       <c r="H15" s="50"/>
@@ -4190,7 +4196,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="147"/>
+      <c r="D16" s="157"/>
       <c r="E16" s="67"/>
       <c r="F16" s="68"/>
       <c r="H16" s="50"/>
@@ -4276,7 +4282,7 @@
       <c r="L23" s="137"/>
     </row>
     <row r="24" spans="2:13" s="78" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="150" t="s">
+      <c r="D24" s="156" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="67"/>
@@ -4287,7 +4293,7 @@
       <c r="L24" s="137"/>
     </row>
     <row r="25" spans="2:13" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="147"/>
+      <c r="D25" s="157"/>
       <c r="E25" s="67"/>
       <c r="F25" s="68"/>
       <c r="H25" s="50"/>
@@ -4296,7 +4302,7 @@
       <c r="L25" s="137"/>
     </row>
     <row r="26" spans="2:13" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="147"/>
+      <c r="D26" s="157"/>
       <c r="E26" s="67"/>
       <c r="F26" s="68"/>
       <c r="H26" s="50"/>
@@ -4305,7 +4311,7 @@
       <c r="L26" s="137"/>
     </row>
     <row r="27" spans="2:13" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="147"/>
+      <c r="D27" s="157"/>
       <c r="E27" s="67"/>
       <c r="F27" s="68"/>
       <c r="H27" s="50"/>
@@ -4591,10 +4597,10 @@
     <row r="45" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="28"/>
       <c r="C45" s="29"/>
-      <c r="D45" s="149" t="s">
+      <c r="D45" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="147"/>
+      <c r="E45" s="157"/>
       <c r="F45" s="16"/>
       <c r="G45" s="7"/>
       <c r="H45" s="50"/>
@@ -4605,10 +4611,10 @@
     <row r="46" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="146" t="s">
+      <c r="D46" s="174" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="147"/>
+      <c r="E46" s="157"/>
       <c r="F46" s="66"/>
       <c r="G46" s="7"/>
       <c r="H46" s="50"/>
@@ -4631,7 +4637,7 @@
     </row>
     <row r="48" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="110"/>
-      <c r="B48" s="157" t="s">
+      <c r="B48" s="159" t="s">
         <v>68</v>
       </c>
       <c r="C48" s="7"/>
@@ -4642,7 +4648,7 @@
         <f>C65</f>
         <v>3</v>
       </c>
-      <c r="F48" s="148" t="s">
+      <c r="F48" s="175" t="s">
         <v>70</v>
       </c>
       <c r="G48" s="7"/>
@@ -4653,7 +4659,7 @@
     </row>
     <row r="49" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="110"/>
-      <c r="B49" s="147"/>
+      <c r="B49" s="157"/>
       <c r="C49" s="7"/>
       <c r="D49" s="14" t="s">
         <v>71</v>
@@ -4662,7 +4668,7 @@
         <f>D65</f>
         <v>9</v>
       </c>
-      <c r="F49" s="147"/>
+      <c r="F49" s="157"/>
       <c r="G49" s="30"/>
       <c r="H49" s="50"/>
       <c r="I49" s="50"/>
@@ -4671,7 +4677,7 @@
     </row>
     <row r="50" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="110"/>
-      <c r="B50" s="147"/>
+      <c r="B50" s="157"/>
       <c r="C50" s="7"/>
       <c r="D50" s="14" t="s">
         <v>72</v>
@@ -4680,7 +4686,7 @@
         <f>B65</f>
         <v>0</v>
       </c>
-      <c r="F50" s="147"/>
+      <c r="F50" s="157"/>
       <c r="G50" s="30"/>
       <c r="H50" s="50"/>
       <c r="I50" s="50"/>
@@ -4689,7 +4695,7 @@
     </row>
     <row r="51" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="110"/>
-      <c r="B51" s="147"/>
+      <c r="B51" s="157"/>
       <c r="C51" s="7"/>
       <c r="D51" s="15" t="s">
         <v>73</v>
@@ -4698,7 +4704,7 @@
         <f>F65</f>
         <v>0</v>
       </c>
-      <c r="F51" s="147"/>
+      <c r="F51" s="157"/>
       <c r="G51" s="30"/>
       <c r="H51" s="50"/>
       <c r="I51" s="50"/>
@@ -4719,13 +4725,13 @@
       <c r="L52" s="137"/>
     </row>
     <row r="53" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="161" t="s">
+      <c r="B53" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="147"/>
-      <c r="D53" s="147"/>
-      <c r="E53" s="147"/>
-      <c r="F53" s="147"/>
+      <c r="C53" s="157"/>
+      <c r="D53" s="157"/>
+      <c r="E53" s="157"/>
+      <c r="F53" s="157"/>
       <c r="G53" s="30"/>
       <c r="H53" s="50"/>
       <c r="I53" s="50"/>
@@ -5063,7 +5069,7 @@
       <c r="H71" s="50"/>
       <c r="I71" s="50"/>
       <c r="J71" s="50"/>
-      <c r="L71" s="173"/>
+      <c r="L71" s="148"/>
     </row>
     <row r="72" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
@@ -5083,7 +5089,7 @@
       <c r="H72" s="50"/>
       <c r="I72" s="50"/>
       <c r="J72" s="50"/>
-      <c r="L72" s="173"/>
+      <c r="L72" s="148"/>
     </row>
     <row r="73" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
@@ -5103,7 +5109,7 @@
       <c r="H73" s="50"/>
       <c r="I73" s="50"/>
       <c r="J73" s="50"/>
-      <c r="L73" s="173"/>
+      <c r="L73" s="148"/>
     </row>
     <row r="74" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="7" t="s">
@@ -5153,10 +5159,10 @@
       <c r="C77" s="87" t="s">
         <v>218</v>
       </c>
-      <c r="D77" s="167" t="s">
+      <c r="D77" s="171" t="s">
         <v>219</v>
       </c>
-      <c r="E77" s="168"/>
+      <c r="E77" s="172"/>
       <c r="F77" s="113"/>
       <c r="G77" s="7"/>
       <c r="L77" s="137"/>
@@ -5164,9 +5170,9 @@
     <row r="78" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
       <c r="C78" s="132"/>
-      <c r="D78" s="174"/>
-      <c r="E78" s="175"/>
-      <c r="F78" s="159" t="s">
+      <c r="D78" s="149"/>
+      <c r="E78" s="150"/>
+      <c r="F78" s="162" t="s">
         <v>99</v>
       </c>
       <c r="G78" s="7"/>
@@ -5178,9 +5184,9 @@
     <row r="79" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="133"/>
-      <c r="D79" s="169"/>
-      <c r="E79" s="170"/>
-      <c r="F79" s="160"/>
+      <c r="D79" s="144"/>
+      <c r="E79" s="145"/>
+      <c r="F79" s="163"/>
       <c r="G79" s="7"/>
       <c r="I79" s="50"/>
       <c r="L79" s="137"/>
@@ -5188,9 +5194,9 @@
     <row r="80" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" s="133"/>
-      <c r="D80" s="169"/>
-      <c r="E80" s="170"/>
-      <c r="F80" s="160"/>
+      <c r="D80" s="144"/>
+      <c r="E80" s="145"/>
+      <c r="F80" s="163"/>
       <c r="G80" s="7"/>
       <c r="I80" s="50"/>
       <c r="L80" s="137"/>
@@ -5198,9 +5204,9 @@
     <row r="81" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
       <c r="C81" s="133"/>
-      <c r="D81" s="169"/>
-      <c r="E81" s="170"/>
-      <c r="F81" s="160"/>
+      <c r="D81" s="144"/>
+      <c r="E81" s="145"/>
+      <c r="F81" s="163"/>
       <c r="G81" s="7"/>
       <c r="I81" s="50"/>
       <c r="L81" s="137"/>
@@ -5208,8 +5214,8 @@
     <row r="82" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
       <c r="C82" s="133"/>
-      <c r="D82" s="169"/>
-      <c r="E82" s="170"/>
+      <c r="D82" s="144"/>
+      <c r="E82" s="145"/>
       <c r="F82" s="113"/>
       <c r="G82" s="7"/>
       <c r="I82" s="50"/>
@@ -5218,8 +5224,8 @@
     <row r="83" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
       <c r="C83" s="133"/>
-      <c r="D83" s="169"/>
-      <c r="E83" s="170"/>
+      <c r="D83" s="144"/>
+      <c r="E83" s="145"/>
       <c r="F83" s="113"/>
       <c r="G83" s="7"/>
       <c r="I83" s="50"/>
@@ -5228,8 +5234,8 @@
     <row r="84" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
       <c r="C84" s="133"/>
-      <c r="D84" s="169"/>
-      <c r="E84" s="170"/>
+      <c r="D84" s="144"/>
+      <c r="E84" s="145"/>
       <c r="F84" s="113"/>
       <c r="G84" s="7"/>
       <c r="I84" s="50"/>
@@ -5238,8 +5244,8 @@
     <row r="85" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" s="133"/>
-      <c r="D85" s="169"/>
-      <c r="E85" s="170"/>
+      <c r="D85" s="144"/>
+      <c r="E85" s="145"/>
       <c r="F85" s="113"/>
       <c r="G85" s="7"/>
       <c r="I85" s="50"/>
@@ -5248,8 +5254,8 @@
     <row r="86" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" s="133"/>
-      <c r="D86" s="169"/>
-      <c r="E86" s="170"/>
+      <c r="D86" s="144"/>
+      <c r="E86" s="145"/>
       <c r="F86" s="113"/>
       <c r="G86" s="7"/>
       <c r="I86" s="50"/>
@@ -5258,8 +5264,8 @@
     <row r="87" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
       <c r="C87" s="133"/>
-      <c r="D87" s="169"/>
-      <c r="E87" s="170"/>
+      <c r="D87" s="144"/>
+      <c r="E87" s="145"/>
       <c r="F87" s="113"/>
       <c r="G87" s="7"/>
       <c r="I87" s="50"/>
@@ -5268,8 +5274,8 @@
     <row r="88" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
       <c r="C88" s="133"/>
-      <c r="D88" s="169"/>
-      <c r="E88" s="170"/>
+      <c r="D88" s="144"/>
+      <c r="E88" s="145"/>
       <c r="F88" s="113"/>
       <c r="G88" s="7"/>
       <c r="I88" s="50"/>
@@ -5278,8 +5284,8 @@
     <row r="89" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
       <c r="C89" s="133"/>
-      <c r="D89" s="169"/>
-      <c r="E89" s="170"/>
+      <c r="D89" s="144"/>
+      <c r="E89" s="145"/>
       <c r="F89" s="113"/>
       <c r="G89" s="7"/>
       <c r="I89" s="50"/>
@@ -5288,8 +5294,8 @@
     <row r="90" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
       <c r="C90" s="133"/>
-      <c r="D90" s="169"/>
-      <c r="E90" s="170"/>
+      <c r="D90" s="144"/>
+      <c r="E90" s="145"/>
       <c r="F90" s="113"/>
       <c r="G90" s="7"/>
       <c r="I90" s="50"/>
@@ -5298,8 +5304,8 @@
     <row r="91" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
       <c r="C91" s="133"/>
-      <c r="D91" s="169"/>
-      <c r="E91" s="170"/>
+      <c r="D91" s="144"/>
+      <c r="E91" s="145"/>
       <c r="F91" s="113"/>
       <c r="G91" s="7"/>
       <c r="I91" s="50"/>
@@ -5308,8 +5314,8 @@
     <row r="92" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
       <c r="C92" s="133"/>
-      <c r="D92" s="169"/>
-      <c r="E92" s="170"/>
+      <c r="D92" s="144"/>
+      <c r="E92" s="145"/>
       <c r="F92" s="113"/>
       <c r="G92" s="7"/>
       <c r="I92" s="50"/>
@@ -5318,8 +5324,8 @@
     <row r="93" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
       <c r="C93" s="133"/>
-      <c r="D93" s="169"/>
-      <c r="E93" s="170"/>
+      <c r="D93" s="144"/>
+      <c r="E93" s="145"/>
       <c r="F93" s="113"/>
       <c r="G93" s="7"/>
       <c r="I93" s="50"/>
@@ -5328,8 +5334,8 @@
     <row r="94" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
       <c r="C94" s="133"/>
-      <c r="D94" s="169"/>
-      <c r="E94" s="170"/>
+      <c r="D94" s="144"/>
+      <c r="E94" s="145"/>
       <c r="F94" s="113"/>
       <c r="G94" s="7"/>
       <c r="I94" s="50"/>
@@ -5338,8 +5344,8 @@
     <row r="95" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="7"/>
       <c r="C95" s="133"/>
-      <c r="D95" s="169"/>
-      <c r="E95" s="170"/>
+      <c r="D95" s="144"/>
+      <c r="E95" s="145"/>
       <c r="F95" s="113"/>
       <c r="G95" s="7"/>
       <c r="I95" s="50"/>
@@ -5348,8 +5354,8 @@
     <row r="96" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="133"/>
-      <c r="D96" s="169"/>
-      <c r="E96" s="170"/>
+      <c r="D96" s="144"/>
+      <c r="E96" s="145"/>
       <c r="F96" s="113"/>
       <c r="G96" s="7"/>
       <c r="I96" s="50"/>
@@ -5358,8 +5364,8 @@
     <row r="97" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="7"/>
       <c r="C97" s="133"/>
-      <c r="D97" s="169"/>
-      <c r="E97" s="170"/>
+      <c r="D97" s="144"/>
+      <c r="E97" s="145"/>
       <c r="F97" s="113"/>
       <c r="G97" s="7"/>
       <c r="I97" s="50"/>
@@ -5368,8 +5374,8 @@
     <row r="98" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="7"/>
       <c r="C98" s="133"/>
-      <c r="D98" s="169"/>
-      <c r="E98" s="170"/>
+      <c r="D98" s="144"/>
+      <c r="E98" s="145"/>
       <c r="F98" s="113"/>
       <c r="G98" s="7"/>
       <c r="I98" s="50"/>
@@ -5378,8 +5384,8 @@
     <row r="99" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="7"/>
       <c r="C99" s="133"/>
-      <c r="D99" s="169"/>
-      <c r="E99" s="170"/>
+      <c r="D99" s="144"/>
+      <c r="E99" s="145"/>
       <c r="F99" s="113"/>
       <c r="G99" s="7"/>
       <c r="I99" s="50"/>
@@ -5388,8 +5394,8 @@
     <row r="100" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="7"/>
       <c r="C100" s="133"/>
-      <c r="D100" s="169"/>
-      <c r="E100" s="170"/>
+      <c r="D100" s="144"/>
+      <c r="E100" s="145"/>
       <c r="F100" s="113"/>
       <c r="G100" s="7"/>
       <c r="I100" s="50"/>
@@ -5398,8 +5404,8 @@
     <row r="101" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="7"/>
       <c r="C101" s="133"/>
-      <c r="D101" s="169"/>
-      <c r="E101" s="170"/>
+      <c r="D101" s="144"/>
+      <c r="E101" s="145"/>
       <c r="F101" s="113"/>
       <c r="G101" s="7"/>
       <c r="I101" s="50"/>
@@ -5408,8 +5414,8 @@
     <row r="102" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="133"/>
-      <c r="D102" s="169"/>
-      <c r="E102" s="170"/>
+      <c r="D102" s="144"/>
+      <c r="E102" s="145"/>
       <c r="F102" s="113"/>
       <c r="G102" s="7"/>
       <c r="I102" s="50"/>
@@ -5418,8 +5424,8 @@
     <row r="103" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="7"/>
       <c r="C103" s="133"/>
-      <c r="D103" s="169"/>
-      <c r="E103" s="170"/>
+      <c r="D103" s="144"/>
+      <c r="E103" s="145"/>
       <c r="F103" s="113"/>
       <c r="G103" s="7"/>
       <c r="I103" s="50"/>
@@ -5428,8 +5434,8 @@
     <row r="104" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
       <c r="C104" s="133"/>
-      <c r="D104" s="169"/>
-      <c r="E104" s="170"/>
+      <c r="D104" s="144"/>
+      <c r="E104" s="145"/>
       <c r="F104" s="113"/>
       <c r="G104" s="7"/>
       <c r="I104" s="50"/>
@@ -5438,8 +5444,8 @@
     <row r="105" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
       <c r="C105" s="133"/>
-      <c r="D105" s="169"/>
-      <c r="E105" s="170"/>
+      <c r="D105" s="144"/>
+      <c r="E105" s="145"/>
       <c r="F105" s="113"/>
       <c r="G105" s="7"/>
       <c r="I105" s="50"/>
@@ -5448,8 +5454,8 @@
     <row r="106" spans="2:12" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
       <c r="C106" s="133"/>
-      <c r="D106" s="169"/>
-      <c r="E106" s="170"/>
+      <c r="D106" s="144"/>
+      <c r="E106" s="145"/>
       <c r="F106" s="113"/>
       <c r="G106" s="7"/>
       <c r="I106" s="50"/>
@@ -5458,8 +5464,8 @@
     <row r="107" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="7"/>
       <c r="C107" s="133"/>
-      <c r="D107" s="169"/>
-      <c r="E107" s="170"/>
+      <c r="D107" s="144"/>
+      <c r="E107" s="145"/>
       <c r="F107" s="114"/>
       <c r="G107" s="7"/>
       <c r="H107" s="50"/>
@@ -5471,8 +5477,8 @@
     <row r="108" spans="2:12" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
       <c r="C108" s="134"/>
-      <c r="D108" s="171"/>
-      <c r="E108" s="172"/>
+      <c r="D108" s="146"/>
+      <c r="E108" s="147"/>
       <c r="F108" s="114"/>
       <c r="G108" s="7"/>
       <c r="H108" s="50"/>
@@ -5506,8 +5512,8 @@
       <c r="E110" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="F110" s="72">
-        <v>10</v>
+      <c r="F110" s="176" t="s">
+        <v>220</v>
       </c>
       <c r="G110" s="72"/>
       <c r="H110" s="50"/>
@@ -5935,11 +5941,11 @@
       <c r="C136" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D136" s="158" t="s">
+      <c r="D136" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="E136" s="145"/>
-      <c r="F136" s="145"/>
+      <c r="E136" s="161"/>
+      <c r="F136" s="161"/>
       <c r="G136" s="81"/>
       <c r="H136" s="50"/>
       <c r="I136" s="50"/>
@@ -6498,7 +6504,7 @@
     <row r="175" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B175" s="42"/>
       <c r="C175" s="83"/>
-      <c r="D175" s="166" t="s">
+      <c r="D175" s="170" t="s">
         <v>118</v>
       </c>
       <c r="E175" s="153"/>
@@ -6742,10 +6748,10 @@
     <row r="189" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B189" s="28"/>
       <c r="C189" s="29"/>
-      <c r="D189" s="149" t="s">
+      <c r="D189" s="165" t="s">
         <v>147</v>
       </c>
-      <c r="E189" s="145"/>
+      <c r="E189" s="161"/>
       <c r="F189" s="29"/>
       <c r="G189" s="29"/>
       <c r="H189" s="55"/>
@@ -6858,7 +6864,7 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="120"/>
-      <c r="B198" s="165" t="s">
+      <c r="B198" s="169" t="s">
         <v>151</v>
       </c>
       <c r="C198" s="152"/>
@@ -6911,10 +6917,10 @@
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B202" s="33"/>
       <c r="C202" s="126"/>
-      <c r="D202" s="163" t="s">
+      <c r="D202" s="167" t="s">
         <v>152</v>
       </c>
-      <c r="E202" s="164"/>
+      <c r="E202" s="168"/>
       <c r="F202" s="126"/>
       <c r="G202" s="126"/>
       <c r="H202" s="56"/>
@@ -6923,7 +6929,7 @@
       <c r="L202" s="135"/>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B203" s="162" t="s">
+      <c r="B203" s="166" t="s">
         <v>153</v>
       </c>
       <c r="C203" s="152"/>
@@ -7264,6 +7270,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="B222:F223"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="D136:F136"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="B219:F220"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="D202:E202"/>
+    <mergeCell ref="B198:F199"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="D108:E108"/>
     <mergeCell ref="L71:L73"/>
@@ -7280,42 +7322,6 @@
     <mergeCell ref="D104:E104"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="B222:F223"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="D136:F136"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="B219:F220"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="D202:E202"/>
-    <mergeCell ref="B198:F199"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <conditionalFormatting sqref="B3 H183:H184 J183:J184">
     <cfRule type="cellIs" dxfId="166" priority="236" stopIfTrue="1" operator="lessThan">

</xml_diff>